<commit_message>
Pooh Points: normal 20260131
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-01-31.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-01-31.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V74"/>
+  <dimension ref="A1:V76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="17" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -597,17 +597,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H2" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2" t="n">
         <v>14</v>
       </c>
-      <c r="I2" t="n">
-        <v>12</v>
-      </c>
       <c r="J2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K2" t="n">
         <v>2</v>
@@ -628,10 +628,10 @@
         <v>24</v>
       </c>
       <c r="Q2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -679,7 +679,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -707,7 +707,7 @@
         <v>3</v>
       </c>
       <c r="P3" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q3" t="n">
         <v>5</v>
@@ -761,7 +761,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -1089,17 +1089,17 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I8" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -1114,22 +1114,22 @@
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="Q8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
@@ -1253,11 +1253,11 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I10" t="n">
         <v>23</v>
@@ -1281,19 +1281,19 @@
         <v>1</v>
       </c>
       <c r="P10" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q10" t="n">
         <v>9</v>
       </c>
       <c r="R10" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S10" t="n">
         <v>3</v>
       </c>
       <c r="T10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U10" t="n">
         <v>2</v>
@@ -1335,14 +1335,14 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>8</v>
       </c>
       <c r="I11" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -1357,25 +1357,25 @@
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>4</v>
+      </c>
+      <c r="R11" t="n">
         <v>6</v>
       </c>
-      <c r="Q11" t="n">
-        <v>3</v>
-      </c>
-      <c r="R11" t="n">
-        <v>4</v>
-      </c>
       <c r="S11" t="n">
         <v>1</v>
       </c>
       <c r="T11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11" t="n">
         <v>2</v>
@@ -1417,17 +1417,17 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I12" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="n">
         <v>2</v>
@@ -1445,13 +1445,13 @@
         <v>1</v>
       </c>
       <c r="P12" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="Q12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R12" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S12" t="n">
         <v>1</v>
@@ -1463,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -1499,11 +1499,11 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I13" t="n">
         <v>9</v>
@@ -1515,7 +1515,7 @@
         <v>3</v>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
@@ -1527,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="P13" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q13" t="n">
         <v>4</v>
@@ -1581,35 +1581,35 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="Q14" t="n">
         <v>0</v>
@@ -1624,10 +1624,10 @@
         <v>0</v>
       </c>
       <c r="U14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -1745,20 +1745,20 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
@@ -1773,25 +1773,25 @@
         <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1827,14 +1827,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J17" t="n">
         <v>1</v>
@@ -1843,7 +1843,7 @@
         <v>2</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" t="n">
         <v>0</v>
@@ -1855,13 +1855,13 @@
         <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1870,10 +1870,10 @@
         <v>2</v>
       </c>
       <c r="U17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V17" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -2073,11 +2073,11 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I20" t="n">
         <v>15</v>
@@ -2101,19 +2101,19 @@
         <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q20" t="n">
         <v>6</v>
       </c>
       <c r="R20" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="S20" t="n">
         <v>3</v>
       </c>
       <c r="T20" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -2304,12 +2304,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Jeff Nwankwo</t>
+          <t>Jordan Pope</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2319,53 +2319,53 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H23" t="n">
+        <v>6</v>
+      </c>
+      <c r="I23" t="n">
+        <v>12</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1</v>
+      </c>
+      <c r="P23" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q23" t="n">
         <v>4</v>
       </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" t="n">
-        <v>3</v>
-      </c>
-      <c r="K23" t="n">
-        <v>1</v>
-      </c>
-      <c r="L23" t="n">
-        <v>2</v>
-      </c>
-      <c r="M23" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" t="n">
-        <v>2</v>
-      </c>
-      <c r="P23" t="n">
-        <v>13</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -2386,12 +2386,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Jordan Pope</t>
+          <t>Jeff Nwankwo</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2401,53 +2401,53 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I24" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M24" t="n">
         <v>0</v>
       </c>
       <c r="N24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P24" t="n">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="Q24" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R24" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="S24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T24" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="U24" t="n">
         <v>0</v>
       </c>
       <c r="V24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -2493,7 +2493,7 @@
         <v>18</v>
       </c>
       <c r="J25" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K25" t="n">
         <v>6</v>
@@ -2505,16 +2505,16 @@
         <v>0</v>
       </c>
       <c r="N25" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O25" t="n">
         <v>1</v>
       </c>
       <c r="P25" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R25" t="n">
         <v>9</v>
@@ -2526,10 +2526,10 @@
         <v>1</v>
       </c>
       <c r="U25" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="V25" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H30" t="n">
@@ -2975,23 +2975,23 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="I31" t="n">
         <v>2</v>
       </c>
       <c r="J31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K31" t="n">
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" t="n">
         <v>0</v>
@@ -3003,19 +3003,19 @@
         <v>1</v>
       </c>
       <c r="P31" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>1</v>
+      </c>
+      <c r="R31" t="n">
         <v>8</v>
       </c>
-      <c r="Q31" t="n">
-        <v>1</v>
-      </c>
-      <c r="R31" t="n">
-        <v>3</v>
-      </c>
       <c r="S31" t="n">
         <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U31" t="n">
         <v>0</v>
@@ -3221,17 +3221,17 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" t="n">
         <v>2</v>
       </c>
       <c r="J34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K34" t="n">
         <v>0</v>
@@ -3246,7 +3246,7 @@
         <v>1</v>
       </c>
       <c r="O34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P34" t="n">
         <v>24</v>
@@ -3467,7 +3467,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H37" t="n">
@@ -3477,7 +3477,7 @@
         <v>8</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" t="n">
         <v>0</v>
@@ -3489,13 +3489,13 @@
         <v>0</v>
       </c>
       <c r="N37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P37" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="Q37" t="n">
         <v>2</v>
@@ -3698,68 +3698,68 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Ali Dibba</t>
+          <t>T.O. Barrett</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>TA&amp;M@UGA</t>
+          <t>MSST@MIZ</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I40" t="n">
+        <v>12</v>
+      </c>
+      <c r="J40" t="n">
+        <v>3</v>
+      </c>
+      <c r="K40" t="n">
+        <v>2</v>
+      </c>
+      <c r="L40" t="n">
+        <v>1</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>1</v>
+      </c>
+      <c r="O40" t="n">
+        <v>1</v>
+      </c>
+      <c r="P40" t="n">
         <v>15</v>
       </c>
-      <c r="J40" t="n">
-        <v>2</v>
-      </c>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" t="n">
-        <v>1</v>
-      </c>
-      <c r="M40" t="n">
-        <v>1</v>
-      </c>
-      <c r="N40" t="n">
-        <v>1</v>
-      </c>
-      <c r="O40" t="n">
-        <v>2</v>
-      </c>
-      <c r="P40" t="n">
-        <v>19</v>
-      </c>
       <c r="Q40" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="R40" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="S40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T40" t="n">
+        <v>3</v>
+      </c>
+      <c r="U40" t="n">
         <v>4</v>
       </c>
-      <c r="U40" t="n">
-        <v>0</v>
-      </c>
       <c r="V40" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -3780,35 +3780,35 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Chendall Weaver</t>
+          <t>Ali Dibba</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>TEX@OU</t>
+          <t>TA&amp;M@UGA</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H41" t="n">
         <v>14</v>
       </c>
       <c r="I41" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J41" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K41" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L41" t="n">
         <v>1</v>
@@ -3820,28 +3820,28 @@
         <v>1</v>
       </c>
       <c r="O41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P41" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q41" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R41" t="n">
+        <v>10</v>
+      </c>
+      <c r="S41" t="n">
+        <v>3</v>
+      </c>
+      <c r="T41" t="n">
         <v>4</v>
       </c>
-      <c r="S41" t="n">
-        <v>1</v>
-      </c>
-      <c r="T41" t="n">
-        <v>2</v>
-      </c>
       <c r="U41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V41" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -3862,56 +3862,56 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Elijah Strong</t>
+          <t>Chendall Weaver</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>LSU@SC</t>
+          <t>TEX@OU</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Final/OT</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H42" t="n">
         <v>14</v>
       </c>
       <c r="I42" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J42" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K42" t="n">
         <v>2</v>
       </c>
       <c r="L42" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N42" t="n">
         <v>1</v>
       </c>
       <c r="O42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P42" t="n">
         <v>23</v>
       </c>
       <c r="Q42" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R42" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="S42" t="n">
         <v>1</v>
@@ -3923,7 +3923,7 @@
         <v>1</v>
       </c>
       <c r="V42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -3944,38 +3944,38 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Camden Heide</t>
+          <t>Elijah Strong</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>TEX@OU</t>
+          <t>LSU@SC</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final/OT</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I43" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J43" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L43" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M43" t="n">
         <v>0</v>
@@ -3984,28 +3984,28 @@
         <v>1</v>
       </c>
       <c r="O43" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P43" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q43" t="n">
         <v>5</v>
       </c>
       <c r="R43" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="S43" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T43" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V43" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -4026,35 +4026,35 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Eli Ellis</t>
+          <t>Camden Heide</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>LSU@SC</t>
+          <t>TEX@OU</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Final/OT</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H44" t="n">
         <v>13</v>
       </c>
       <c r="I44" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J44" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K44" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L44" t="n">
         <v>0</v>
@@ -4063,31 +4063,31 @@
         <v>0</v>
       </c>
       <c r="N44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O44" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P44" t="n">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="Q44" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R44" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="S44" t="n">
         <v>3</v>
       </c>
       <c r="T44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U44" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V44" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -4108,41 +4108,41 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Simeon Wilcher</t>
+          <t>Eli Ellis</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>TEX@OU</t>
+          <t>LSU@SC</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final/OT</t>
         </is>
       </c>
       <c r="H45" t="n">
         <v>13</v>
       </c>
       <c r="I45" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45" t="n">
         <v>0</v>
@@ -4151,25 +4151,25 @@
         <v>2</v>
       </c>
       <c r="P45" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="Q45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R45" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="S45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T45" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U45" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V45" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46">
@@ -4190,17 +4190,17 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Pop Isaacs</t>
+          <t>Simeon Wilcher</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>TA&amp;M@UGA</t>
+          <t>TEX@OU</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -4209,49 +4209,49 @@
         </is>
       </c>
       <c r="H46" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I46" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J46" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L46" t="n">
         <v>1</v>
       </c>
       <c r="M46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P46" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="Q46" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R46" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T46" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -4272,35 +4272,35 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Robert Miller III</t>
+          <t>Pop Isaacs</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>LSU@SC</t>
+          <t>TA&amp;M@UGA</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Final/OT</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H47" t="n">
         <v>12</v>
       </c>
       <c r="I47" t="n">
+        <v>11</v>
+      </c>
+      <c r="J47" t="n">
         <v>6</v>
       </c>
-      <c r="J47" t="n">
-        <v>5</v>
-      </c>
       <c r="K47" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L47" t="n">
         <v>1</v>
@@ -4312,28 +4312,28 @@
         <v>1</v>
       </c>
       <c r="O47" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P47" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="Q47" t="n">
         <v>3</v>
       </c>
       <c r="R47" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="S47" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T47" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -4354,68 +4354,68 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Jacari Lane</t>
+          <t>Robert Miller III</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>TA&amp;M@UGA</t>
+          <t>LSU@SC</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>Final/OT</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I48" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J48" t="n">
+        <v>5</v>
+      </c>
+      <c r="K48" t="n">
+        <v>3</v>
+      </c>
+      <c r="L48" t="n">
+        <v>1</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" t="n">
+        <v>1</v>
+      </c>
+      <c r="O48" t="n">
         <v>4</v>
       </c>
-      <c r="K48" t="n">
-        <v>3</v>
-      </c>
-      <c r="L48" t="n">
-        <v>1</v>
-      </c>
-      <c r="M48" t="n">
-        <v>0</v>
-      </c>
-      <c r="N48" t="n">
-        <v>3</v>
-      </c>
-      <c r="O48" t="n">
-        <v>3</v>
-      </c>
       <c r="P48" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Q48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T48" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U48" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V48" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -4436,12 +4436,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Kanon Catchings</t>
+          <t>Jacari Lane</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4458,46 +4458,46 @@
         <v>10</v>
       </c>
       <c r="I49" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K49" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49" t="n">
         <v>0</v>
       </c>
       <c r="N49" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O49" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P49" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="Q49" t="n">
+        <v>2</v>
+      </c>
+      <c r="R49" t="n">
         <v>6</v>
       </c>
-      <c r="R49" t="n">
-        <v>14</v>
-      </c>
       <c r="S49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T49" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U49" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V49" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -4518,68 +4518,68 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>T.O. Barrett</t>
+          <t>Kanon Catchings</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>MIZ</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>MSST@MIZ</t>
+          <t>TA&amp;M@UGA</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H50" t="n">
         <v>10</v>
       </c>
       <c r="I50" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J50" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M50" t="n">
         <v>0</v>
       </c>
       <c r="N50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P50" t="n">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="Q50" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R50" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="S50" t="n">
         <v>2</v>
       </c>
       <c r="T50" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="U50" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V50" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -4615,7 +4615,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H51" t="n">
@@ -4640,10 +4640,10 @@
         <v>0</v>
       </c>
       <c r="O51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P51" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q51" t="n">
         <v>1</v>
@@ -4764,38 +4764,38 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Trent Pierce</t>
+          <t>Jordan Ross</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>MIZ</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>MSST@MIZ</t>
+          <t>TA&amp;M@UGA</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I53" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J53" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K53" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L53" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M53" t="n">
         <v>0</v>
@@ -4807,25 +4807,25 @@
         <v>2</v>
       </c>
       <c r="P53" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="Q53" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S53" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V53" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -4846,68 +4846,68 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Jordan Ross</t>
+          <t>Trent Pierce</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>TA&amp;M@UGA</t>
+          <t>MSST@MIZ</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H54" t="n">
         <v>7</v>
       </c>
       <c r="I54" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J54" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="n">
+        <v>2</v>
+      </c>
+      <c r="P54" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>3</v>
+      </c>
+      <c r="R54" t="n">
+        <v>5</v>
+      </c>
+      <c r="S54" t="n">
+        <v>2</v>
+      </c>
+      <c r="T54" t="n">
         <v>4</v>
       </c>
-      <c r="L54" t="n">
-        <v>2</v>
-      </c>
-      <c r="M54" t="n">
-        <v>0</v>
-      </c>
-      <c r="N54" t="n">
-        <v>0</v>
-      </c>
-      <c r="O54" t="n">
-        <v>2</v>
-      </c>
-      <c r="P54" t="n">
-        <v>17</v>
-      </c>
-      <c r="Q54" t="n">
-        <v>0</v>
-      </c>
-      <c r="R54" t="n">
-        <v>2</v>
-      </c>
-      <c r="S54" t="n">
-        <v>0</v>
-      </c>
-      <c r="T54" t="n">
-        <v>1</v>
-      </c>
       <c r="U54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V54" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -5010,62 +5010,62 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Grant Polk</t>
+          <t>Shawn Phillips Jr.</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>LSU@SC</t>
+          <t>MSST@MIZ</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Final/OT</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H56" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I56" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" t="n">
         <v>0</v>
       </c>
       <c r="M56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P56" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q56" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R56" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S56" t="n">
         <v>0</v>
       </c>
       <c r="T56" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U56" t="n">
         <v>0</v>
@@ -5092,38 +5092,38 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Josh Holloway</t>
+          <t>Grant Polk</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>TA&amp;M@UGA</t>
+          <t>LSU@SC</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>Final/OT</t>
         </is>
       </c>
       <c r="H57" t="n">
         <v>5</v>
       </c>
       <c r="I57" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J57" t="n">
         <v>3</v>
       </c>
       <c r="K57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M57" t="n">
         <v>0</v>
@@ -5135,25 +5135,25 @@
         <v>1</v>
       </c>
       <c r="P57" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Q57" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R57" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S57" t="n">
         <v>0</v>
       </c>
       <c r="T57" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U57" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V57" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -5174,38 +5174,38 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>King Grace</t>
+          <t>Josh Holloway</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>MSST</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>MSST@MIZ</t>
+          <t>TA&amp;M@UGA</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H58" t="n">
         <v>5</v>
       </c>
       <c r="I58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J58" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M58" t="n">
         <v>0</v>
@@ -5214,28 +5214,28 @@
         <v>0</v>
       </c>
       <c r="O58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P58" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="Q58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U58" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V58" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -5256,68 +5256,68 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>PJ Carter</t>
+          <t>Achor Achor</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>MSST</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>LSU@SC</t>
+          <t>MSST@MIZ</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Final/OT</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H59" t="n">
         <v>4</v>
       </c>
       <c r="I59" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J59" t="n">
         <v>1</v>
       </c>
       <c r="K59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L59" t="n">
         <v>0</v>
       </c>
       <c r="M59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P59" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="Q59" t="n">
         <v>2</v>
       </c>
       <c r="R59" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="S59" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T59" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="U59" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V59" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -5338,68 +5338,68 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Achor Achor</t>
+          <t>PJ Carter</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>MSST</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>MSST@MIZ</t>
+          <t>LSU@SC</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>Final/OT</t>
         </is>
       </c>
       <c r="H60" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I60" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J60" t="n">
         <v>1</v>
       </c>
       <c r="K60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60" t="n">
         <v>0</v>
       </c>
       <c r="M60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P60" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="Q60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R60" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="S60" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T60" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U60" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V60" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
@@ -5420,68 +5420,68 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>EJ Walker</t>
+          <t>Sergej Macura</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>MSST</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>LSU@SC</t>
+          <t>MSST@MIZ</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Final/OT</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H61" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I61" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K61" t="n">
         <v>0</v>
       </c>
       <c r="L61" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M61" t="n">
         <v>0</v>
       </c>
       <c r="N61" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O61" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P61" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="Q61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R61" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S61" t="n">
         <v>0</v>
       </c>
       <c r="T61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V61" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -5502,29 +5502,29 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Justin Abson</t>
+          <t>King Grace</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>MSST</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>TA&amp;M@UGA</t>
+          <t>MSST@MIZ</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H62" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I62" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J62" t="n">
         <v>2</v>
@@ -5539,25 +5539,25 @@
         <v>0</v>
       </c>
       <c r="N62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U62" t="n">
         <v>0</v>
@@ -5584,41 +5584,41 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Kareem Stagg</t>
+          <t>EJ Walker</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>TA&amp;M@UGA</t>
+          <t>LSU@SC</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>Final/OT</t>
         </is>
       </c>
       <c r="H63" t="n">
         <v>2</v>
       </c>
       <c r="I63" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J63" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K63" t="n">
         <v>0</v>
       </c>
       <c r="L63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N63" t="n">
         <v>2</v>
@@ -5627,13 +5627,13 @@
         <v>2</v>
       </c>
       <c r="P63" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Q63" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R63" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S63" t="n">
         <v>0</v>
@@ -5642,10 +5642,10 @@
         <v>1</v>
       </c>
       <c r="U63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V63" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -5666,12 +5666,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Shawn Phillips Jr.</t>
+          <t>Jamarion Davis-Fleming</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>MIZ</t>
+          <t>MSST</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H64" t="n">
@@ -5691,25 +5691,25 @@
         <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L64" t="n">
         <v>0</v>
       </c>
       <c r="M64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P64" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="Q64" t="n">
         <v>0</v>
@@ -5727,7 +5727,7 @@
         <v>0</v>
       </c>
       <c r="V64" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -5748,12 +5748,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Federiko Federiko</t>
+          <t>Justin Abson</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5767,13 +5767,13 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I65" t="n">
         <v>0</v>
       </c>
       <c r="J65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K65" t="n">
         <v>0</v>
@@ -5791,7 +5791,7 @@
         <v>0</v>
       </c>
       <c r="P65" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q65" t="n">
         <v>0</v>
@@ -5830,62 +5830,62 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Hayden Assemian</t>
+          <t>Kareem Stagg</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>LSU@SC</t>
+          <t>TA&amp;M@UGA</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Final/OT</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I66" t="n">
         <v>0</v>
       </c>
       <c r="J66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K66" t="n">
         <v>0</v>
       </c>
       <c r="L66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P66" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Q66" t="n">
         <v>0</v>
       </c>
       <c r="R66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
       </c>
       <c r="T66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U66" t="n">
         <v>0</v>
@@ -5927,11 +5927,11 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I67" t="n">
         <v>0</v>
@@ -5946,7 +5946,7 @@
         <v>1</v>
       </c>
       <c r="M67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N67" t="n">
         <v>2</v>
@@ -5955,7 +5955,7 @@
         <v>1</v>
       </c>
       <c r="P67" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q67" t="n">
         <v>0</v>
@@ -5994,22 +5994,22 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Sergej Macura</t>
+          <t>Federiko Federiko</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>MSST</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>MSST@MIZ</t>
+          <t>TA&amp;M@UGA</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H68" t="n">
@@ -6037,7 +6037,7 @@
         <v>0</v>
       </c>
       <c r="P68" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q68" t="n">
         <v>0</v>
@@ -6076,32 +6076,32 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Zach Clemence</t>
+          <t>Hayden Assemian</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>TA&amp;M@UGA</t>
+          <t>LSU@SC</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>Final/OT</t>
         </is>
       </c>
       <c r="H69" t="n">
         <v>1</v>
       </c>
       <c r="I69" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K69" t="n">
         <v>0</v>
@@ -6116,28 +6116,28 @@
         <v>0</v>
       </c>
       <c r="O69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P69" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q69" t="n">
         <v>0</v>
       </c>
       <c r="R69" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S69" t="n">
         <v>0</v>
       </c>
       <c r="T69" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U69" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V69" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -6158,35 +6158,35 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Ja'Borri McGhee</t>
+          <t>Zach Clemence</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>MSST</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>MSST@MIZ</t>
+          <t>TA&amp;M@UGA</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" t="n">
         <v>2</v>
       </c>
       <c r="J70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K70" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L70" t="n">
         <v>0</v>
@@ -6195,31 +6195,31 @@
         <v>0</v>
       </c>
       <c r="N70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P70" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S70" t="n">
         <v>0</v>
       </c>
       <c r="T70" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -6240,12 +6240,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Jamarion Davis-Fleming</t>
+          <t>Annor Boateng</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>MSST</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6255,7 +6255,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H71" t="n">
@@ -6265,7 +6265,7 @@
         <v>0</v>
       </c>
       <c r="J71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K71" t="n">
         <v>0</v>
@@ -6277,13 +6277,13 @@
         <v>0</v>
       </c>
       <c r="N71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O71" t="n">
         <v>0</v>
       </c>
       <c r="P71" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q71" t="n">
         <v>0</v>
@@ -6301,7 +6301,7 @@
         <v>0</v>
       </c>
       <c r="V71" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -6337,7 +6337,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>6:27 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H72" t="n">
@@ -6419,7 +6419,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>12:47 - 1st Half</t>
+          <t>4:14 - 1st Half</t>
         </is>
       </c>
       <c r="H73" t="n">
@@ -6447,7 +6447,7 @@
         <v>0</v>
       </c>
       <c r="P73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q73" t="n">
         <v>0</v>
@@ -6486,67 +6486,231 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
+          <t>Trent Burns</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>MIZ</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>MSST@MIZ</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>4:14 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="n">
+        <v>0</v>
+      </c>
+      <c r="P74" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>0</v>
+      </c>
+      <c r="R74" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" t="n">
+        <v>0</v>
+      </c>
+      <c r="T74" t="n">
+        <v>0</v>
+      </c>
+      <c r="U74" t="n">
+        <v>0</v>
+      </c>
+      <c r="V74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Ja'Borri McGhee</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>MSST</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>MSST@MIZ</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>4:14 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I75" t="n">
+        <v>3</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="n">
+        <v>2</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0</v>
+      </c>
+      <c r="M75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N75" t="n">
+        <v>1</v>
+      </c>
+      <c r="O75" t="n">
+        <v>0</v>
+      </c>
+      <c r="P75" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>1</v>
+      </c>
+      <c r="R75" t="n">
+        <v>5</v>
+      </c>
+      <c r="S75" t="n">
+        <v>0</v>
+      </c>
+      <c r="T75" t="n">
+        <v>2</v>
+      </c>
+      <c r="U75" t="n">
+        <v>1</v>
+      </c>
+      <c r="V75" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
           <t>Justin Bailey</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="E76" t="inlineStr">
         <is>
           <t>UGA</t>
         </is>
       </c>
-      <c r="F74" t="inlineStr">
+      <c r="F76" t="inlineStr">
         <is>
           <t>TA&amp;M@UGA</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr">
+      <c r="G76" t="inlineStr">
         <is>
           <t>Final</t>
         </is>
       </c>
-      <c r="H74" t="n">
+      <c r="H76" t="n">
         <v>-1</v>
       </c>
-      <c r="I74" t="n">
-        <v>2</v>
-      </c>
-      <c r="J74" t="n">
-        <v>0</v>
-      </c>
-      <c r="K74" t="n">
-        <v>0</v>
-      </c>
-      <c r="L74" t="n">
-        <v>1</v>
-      </c>
-      <c r="M74" t="n">
-        <v>0</v>
-      </c>
-      <c r="N74" t="n">
-        <v>1</v>
-      </c>
-      <c r="O74" t="n">
+      <c r="I76" t="n">
+        <v>2</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L76" t="n">
+        <v>1</v>
+      </c>
+      <c r="M76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N76" t="n">
+        <v>1</v>
+      </c>
+      <c r="O76" t="n">
         <v>4</v>
       </c>
-      <c r="P74" t="n">
+      <c r="P76" t="n">
         <v>9</v>
       </c>
-      <c r="Q74" t="n">
-        <v>1</v>
-      </c>
-      <c r="R74" t="n">
+      <c r="Q76" t="n">
+        <v>1</v>
+      </c>
+      <c r="R76" t="n">
         <v>4</v>
       </c>
-      <c r="S74" t="n">
-        <v>0</v>
-      </c>
-      <c r="T74" t="n">
-        <v>1</v>
-      </c>
-      <c r="U74" t="n">
-        <v>0</v>
-      </c>
-      <c r="V74" t="n">
+      <c r="S76" t="n">
+        <v>0</v>
+      </c>
+      <c r="T76" t="n">
+        <v>1</v>
+      </c>
+      <c r="U76" t="n">
+        <v>0</v>
+      </c>
+      <c r="V76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6598,7 +6762,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" t="n">
         <v>3</v>
@@ -6611,7 +6775,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C3" t="n">
         <v>3</v>
@@ -6633,27 +6797,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>The Backslashers</t>
+          <t>Three Dawg Nite</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Three Dawg Nite</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -6663,7 +6827,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" t="n">
         <v>2</v>
@@ -6676,7 +6840,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>

</xml_diff>